<commit_message>
i think it works
</commit_message>
<xml_diff>
--- a/excel_stuff/Book2.xlsx
+++ b/excel_stuff/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\PycharmProjects\mathias\Python\excel_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F191393-DB8C-4B74-AE94-88C1445CEEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC15760C-A89C-4231-A3F3-78267DAC6245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{AF37207D-5B49-481F-89A9-5842FEB4CE75}"/>
+    <workbookView xWindow="6675" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{AF37207D-5B49-481F-89A9-5842FEB4CE75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,139 +371,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB81AF7-0585-4AA2-B633-FC611D1CE587}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="B1">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>308</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>307</v>
       </c>
-      <c r="C6">
+      <c r="B6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>306</v>
       </c>
-      <c r="C7">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>305</v>
       </c>
-      <c r="C8">
+      <c r="B8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="B9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="C11">
+      <c r="B11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>308</v>
       </c>
-      <c r="C13">
+      <c r="B13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>307</v>
       </c>
-      <c r="C14">
+      <c r="B14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>306</v>
       </c>
-      <c r="C15">
+      <c r="B15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>305</v>
       </c>
-      <c r="C16">
+      <c r="B16">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Expanded to include 10 columns
</commit_message>
<xml_diff>
--- a/excel_stuff/Book2.xlsx
+++ b/excel_stuff/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\PycharmProjects\mathias\Python\excel_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC15760C-A89C-4231-A3F3-78267DAC6245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7E0357-3E40-4D35-90F3-36D3096EF66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6675" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{AF37207D-5B49-481F-89A9-5842FEB4CE75}"/>
   </bookViews>
@@ -22,6 +22,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="8">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,140 +400,524 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB81AF7-0585-4AA2-B633-FC611D1CE587}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>308</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>307</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>306</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>305</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>308</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>307</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>306</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>305</v>
       </c>
       <c r="B16">
         <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>